<commit_message>
Created Mark1, and also made some code for it
</commit_message>
<xml_diff>
--- a/Excel and Maths/AutonomousAlgorithm.xlsx
+++ b/Excel and Maths/AutonomousAlgorithm.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863CC186-4471-49B7-9BC5-2D6536B7B68C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4688176B-5728-436F-9332-9A2890886E87}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1379,15 +1379,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1681,7 +1681,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added More Stuff to Excel Spreadsheet
</commit_message>
<xml_diff>
--- a/Excel and Maths/AutonomousAlgorithm.xlsx
+++ b/Excel and Maths/AutonomousAlgorithm.xlsx
@@ -3,13 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4688176B-5728-436F-9332-9A2890886E87}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB5E090-48F1-4089-BBE7-AA3EFEF7BEEF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ContantsAndEquation" sheetId="1" r:id="rId1"/>
+    <sheet name="Test1 - Consitency" sheetId="2" r:id="rId2"/>
+    <sheet name="Test2 - Distance Relationship" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Test1 - Consitency'!$B$2:$B$50</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Test1 - Consitency'!$B$2:$B$50</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <r>
       <t>V</t>
@@ -238,6 +244,42 @@
       <t>(Output)</t>
     </r>
   </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Distance (in)</t>
+  </si>
+  <si>
+    <t>26.132x-52.912</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>IQR</t>
+  </si>
 </sst>
 </file>
 
@@ -312,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -325,6 +367,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,34 +485,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -481,37 +524,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.19999999999999996</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41599999999999998</c:v>
+                  <c:v>0.48000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.58400000000000007</c:v>
+                  <c:v>0.62000000000000011</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.70400000000000007</c:v>
+                  <c:v>0.72000000000000008</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.77600000000000002</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.77600000000000002</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.70400000000000007</c:v>
+                  <c:v>0.72000000000000008</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.58400000000000007</c:v>
+                  <c:v>0.62000000000000011</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.41599999999999998</c:v>
+                  <c:v>0.48000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.19999999999999996</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -818,7 +861,588 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.0877461407371471E-2"/>
+                  <c:y val="-0.16390018955963837"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Test2 - Distance Relationship'!$A$2:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Test2 - Distance Relationship'!$B$2:$B$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-47EF-42B7-8A11-BA40EE27C34B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="765126384"/>
+        <c:axId val="625300128"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="765126384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="625300128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="625300128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="765126384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Box Plot</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Box Plot</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{E310C388-F5AF-4176-AC96-76F98EE1A2D9}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1374,6 +1998,1037 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1395,6 +3050,130 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9184C67F-CE12-4542-BF00-27C38ACCEDE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>490537</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>185737</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Chart 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A5F2F49-4877-4F28-B567-DDA57AF1BD0E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3538537" y="0"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D8BD026-489D-4909-B74F-F951A3D42FF9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1680,8 +3459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,7 +3491,7 @@
       </c>
       <c r="E2" s="4">
         <f>(B3-B2)/((B6-(0.5*B7))^2)</f>
-        <v>-2.4000000000000004E-2</v>
+        <v>-0.32</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1720,14 +3499,14 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="4">
         <f>B7/2</f>
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1763,7 +3542,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>9</v>
@@ -1787,53 +3566,53 @@
       </c>
       <c r="B11" s="6">
         <f>(E2*((A11-E3)^2))+B2</f>
-        <v>0.19999999999999996</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <f>A11+(0.1*B7)</f>
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="B12" s="6">
         <f>(E2*((A12-E3)^2))+B2</f>
-        <v>0.41599999999999998</v>
+        <v>0.48000000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <f>A12+(0.1*B7)</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="B13" s="6">
         <f>(E2*((A13-E3)^2))+B2</f>
-        <v>0.58400000000000007</v>
+        <v>0.62000000000000011</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <f>A13+(0.1*B7)</f>
-        <v>3</v>
+        <v>0.75</v>
       </c>
       <c r="B14" s="6">
         <f>(E2*((A14-E3)^2))+B2</f>
-        <v>0.70400000000000007</v>
+        <v>0.72000000000000008</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <f>A14+(0.1*B7)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B15" s="6">
         <f>(E2*((A15-E3)^2))+B2</f>
-        <v>0.77600000000000002</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <f>A15+(0.1*B7)</f>
-        <v>5</v>
+        <v>1.25</v>
       </c>
       <c r="B16" s="6">
         <f>(E2*((A16-E3)^2))+B2</f>
@@ -1843,51 +3622,51 @@
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <f>A16+(0.1*B7)</f>
-        <v>6</v>
+        <v>1.5</v>
       </c>
       <c r="B17" s="6">
         <f>(E2*((A17-E3)^2))+B2</f>
-        <v>0.77600000000000002</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <f>A17+(0.1*B7)</f>
-        <v>7</v>
+        <v>1.75</v>
       </c>
       <c r="B18" s="6">
         <f>(E2*((A18-E3)^2))+B2</f>
-        <v>0.70400000000000007</v>
+        <v>0.72000000000000008</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <f>A18+(0.1*B7)</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B19" s="6">
         <f>(E2*((A19-E3)^2))+B2</f>
-        <v>0.58400000000000007</v>
+        <v>0.62000000000000011</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <f>A19+(0.1*B7)</f>
-        <v>9</v>
+        <v>2.25</v>
       </c>
       <c r="B20" s="6">
         <f>(E2*((A20-E3)^2))+B2</f>
-        <v>0.41599999999999998</v>
+        <v>0.48000000000000004</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <f>A20+(0.1*B7)</f>
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="B21" s="6">
         <f>(E2*((A21-E3)^2))+B2</f>
-        <v>0.19999999999999996</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -1895,4 +3674,355 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1918DEB-34A7-4DC8-88D3-A81E0168A8F1}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1">
+        <f>AVERAGE(B2:B50)</f>
+        <v>77.900000000000006</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>78</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2">
+        <f>MEDIAN(B2:B50)</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>76</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <f>MODE(B2:B50)</f>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>78</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <f>MAX(B2:B50)-MIN(B2:B50)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>77</v>
+      </c>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>79</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <f>QUARTILE(B2:B50,0)</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>79</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <f>QUARTILE(B2:B50,1)</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>77</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <f>QUARTILE(B2:B50,2)</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>77</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9">
+        <f>QUARTILE(B2:B50,3)</f>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>79</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10">
+        <f>QUARTILE(B2:B50,4)</f>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>79</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11">
+        <f>E9-E7</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF22B34-F7DC-419C-8D9C-443AAFEF1F91}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2.5</v>
+      </c>
+      <c r="B2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+0.25</f>
+        <v>2.75</v>
+      </c>
+      <c r="B3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>A3+0.25</f>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>A4+0.25</f>
+        <v>3.25</v>
+      </c>
+      <c r="B5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>A5+0.25</f>
+        <v>3.5</v>
+      </c>
+      <c r="B6">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>A6+0.25</f>
+        <v>3.75</v>
+      </c>
+      <c r="B7">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>A7+0.25</f>
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>A8+0.25</f>
+        <v>4.25</v>
+      </c>
+      <c r="B9">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>A9+0.25</f>
+        <v>4.5</v>
+      </c>
+      <c r="B10">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>A10+0.25</f>
+        <v>4.75</v>
+      </c>
+      <c r="B11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>A11+0.25</f>
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>A12+0.25</f>
+        <v>5.25</v>
+      </c>
+      <c r="B13">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>A13+0.25</f>
+        <v>5.5</v>
+      </c>
+      <c r="B14">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3.3</v>
+      </c>
+      <c r="B15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3.4</v>
+      </c>
+      <c r="B16">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3.6</v>
+      </c>
+      <c r="B17">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3.7</v>
+      </c>
+      <c r="B18">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>